<commit_message>
Working registration with fgusers3
</commit_message>
<xml_diff>
--- a/sql/model.xlsx
+++ b/sql/model.xlsx
@@ -1180,8 +1180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F59" sqref="F59"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>

</xml_diff>